<commit_message>
Test-12 next year KZ (mse)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-12.xlsx
+++ b/migforecasting/underground/test-12.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
   <si>
     <t>test size 20%</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>test (MAPE)</t>
+  </si>
+  <si>
+    <t>train (MSE)</t>
+  </si>
+  <si>
+    <t>test (MSE)</t>
   </si>
 </sst>
 </file>
@@ -99,13 +105,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -388,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:X58"/>
+  <dimension ref="D3:AI58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC35" sqref="AC35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,9 +413,13 @@
     <col min="19" max="19" width="14.5703125" customWidth="1"/>
     <col min="23" max="23" width="14.5703125" customWidth="1"/>
     <col min="24" max="24" width="12.85546875" customWidth="1"/>
+    <col min="29" max="29" width="14.85546875" customWidth="1"/>
+    <col min="30" max="30" width="16.140625" customWidth="1"/>
+    <col min="34" max="34" width="12.85546875" customWidth="1"/>
+    <col min="35" max="35" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:35" x14ac:dyDescent="0.25">
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,8 +432,14 @@
       <c r="W3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AC3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
@@ -437,8 +456,16 @@
         <v>6</v>
       </c>
       <c r="X4" s="1"/>
-    </row>
-    <row r="5" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="1"/>
+      <c r="AG4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="1"/>
+    </row>
+    <row r="5" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
         <v>2</v>
@@ -467,8 +494,22 @@
       <c r="X5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <v>1</v>
       </c>
@@ -505,8 +546,26 @@
       <c r="X6" s="3">
         <v>3.0441390189157111</v>
       </c>
-    </row>
-    <row r="7" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="4">
+        <v>8.7310959796989903E-4</v>
+      </c>
+      <c r="AD6" s="4">
+        <v>5.932368422197627E-3</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="4">
+        <v>1.6285462611402601E-3</v>
+      </c>
+      <c r="AI6" s="4">
+        <v>1.0415924768305921E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <f>D6+1</f>
         <v>2</v>
@@ -547,8 +606,28 @@
       <c r="X7" s="3">
         <v>3.319270880230095</v>
       </c>
-    </row>
-    <row r="8" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB7" s="2">
+        <f>AB6+1</f>
+        <v>2</v>
+      </c>
+      <c r="AC7" s="4">
+        <v>8.7054759684879939E-4</v>
+      </c>
+      <c r="AD7" s="4">
+        <v>5.8219286043002458E-3</v>
+      </c>
+      <c r="AG7" s="2">
+        <f>AG6+1</f>
+        <v>2</v>
+      </c>
+      <c r="AH7" s="4">
+        <v>1.685974050585894E-3</v>
+      </c>
+      <c r="AI7" s="4">
+        <v>1.0244072788939591E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <f t="shared" ref="D8:D55" si="0">D7+1</f>
         <v>3</v>
@@ -589,8 +668,28 @@
       <c r="X8" s="3">
         <v>3.0429507422748552</v>
       </c>
-    </row>
-    <row r="9" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB8" s="2">
+        <f t="shared" ref="AB8:AB55" si="4">AB7+1</f>
+        <v>3</v>
+      </c>
+      <c r="AC8" s="4">
+        <v>8.9078371730447724E-4</v>
+      </c>
+      <c r="AD8" s="4">
+        <v>5.3389520975033553E-3</v>
+      </c>
+      <c r="AG8" s="2">
+        <f t="shared" ref="AG8:AG55" si="5">AG7+1</f>
+        <v>3</v>
+      </c>
+      <c r="AH8" s="4">
+        <v>1.724585444101256E-3</v>
+      </c>
+      <c r="AI8" s="4">
+        <v>9.1566361222046328E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -631,8 +730,28 @@
       <c r="X9" s="3">
         <v>3.4743536146851488</v>
       </c>
-    </row>
-    <row r="10" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB9" s="2">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="AC9" s="4">
+        <v>9.2412889899268051E-4</v>
+      </c>
+      <c r="AD9" s="4">
+        <v>5.9228166490137221E-3</v>
+      </c>
+      <c r="AG9" s="2">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="AH9" s="4">
+        <v>1.6624880913926161E-3</v>
+      </c>
+      <c r="AI9" s="4">
+        <v>1.027152016740329E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -673,8 +792,28 @@
       <c r="X10" s="3">
         <v>3.9373022861239302</v>
       </c>
-    </row>
-    <row r="11" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB10" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="AC10" s="4">
+        <v>9.7348016341827228E-4</v>
+      </c>
+      <c r="AD10" s="4">
+        <v>4.8803194488362374E-3</v>
+      </c>
+      <c r="AG10" s="2">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="AH10" s="4">
+        <v>1.6058960083105919E-3</v>
+      </c>
+      <c r="AI10" s="4">
+        <v>1.157550804482267E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -715,8 +854,28 @@
       <c r="X11" s="3">
         <v>3.433027750186481</v>
       </c>
-    </row>
-    <row r="12" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB11" s="2">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AC11" s="4">
+        <v>9.0423577436433067E-4</v>
+      </c>
+      <c r="AD11" s="4">
+        <v>6.452537677104647E-3</v>
+      </c>
+      <c r="AG11" s="2">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="AH11" s="4">
+        <v>1.5732406876136269E-3</v>
+      </c>
+      <c r="AI11" s="4">
+        <v>1.1944250448709171E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -757,8 +916,28 @@
       <c r="X12" s="3">
         <v>2.638521818088349</v>
       </c>
-    </row>
-    <row r="13" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB12" s="2">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AC12" s="4">
+        <v>8.4642562284647995E-4</v>
+      </c>
+      <c r="AD12" s="4">
+        <v>6.5450990290021006E-3</v>
+      </c>
+      <c r="AG12" s="2">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="AH12" s="4">
+        <v>1.657905539907988E-3</v>
+      </c>
+      <c r="AI12" s="4">
+        <v>1.049765683476319E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -799,8 +978,28 @@
       <c r="X13" s="3">
         <v>3.3299148430581642</v>
       </c>
-    </row>
-    <row r="14" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB13" s="2">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="AC13" s="4">
+        <v>8.6699652935646305E-4</v>
+      </c>
+      <c r="AD13" s="4">
+        <v>7.081593320648184E-3</v>
+      </c>
+      <c r="AG13" s="2">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="AH13" s="4">
+        <v>1.597444438576673E-3</v>
+      </c>
+      <c r="AI13" s="4">
+        <v>1.152936190573064E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -841,8 +1040,28 @@
       <c r="X14" s="3">
         <v>3.6663444691942231</v>
       </c>
-    </row>
-    <row r="15" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB14" s="2">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="AC14" s="4">
+        <v>8.9935724886711869E-4</v>
+      </c>
+      <c r="AD14" s="4">
+        <v>6.712956779829425E-3</v>
+      </c>
+      <c r="AG14" s="2">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="AH14" s="4">
+        <v>1.519713072780016E-3</v>
+      </c>
+      <c r="AI14" s="4">
+        <v>1.3730009994423951E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -883,8 +1102,28 @@
       <c r="X15" s="3">
         <v>3.5705926852768068</v>
       </c>
-    </row>
-    <row r="16" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB15" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="AC15" s="4">
+        <v>9.2270630303479411E-4</v>
+      </c>
+      <c r="AD15" s="4">
+        <v>4.3575756158191082E-3</v>
+      </c>
+      <c r="AG15" s="2">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="AH15" s="4">
+        <v>1.6432642937766349E-3</v>
+      </c>
+      <c r="AI15" s="4">
+        <v>1.1675014975165489E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -925,8 +1164,28 @@
       <c r="X16" s="3">
         <v>3.3682732407575902</v>
       </c>
-    </row>
-    <row r="17" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB16" s="2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="AC16" s="4">
+        <v>7.9329877704101184E-4</v>
+      </c>
+      <c r="AD16" s="4">
+        <v>7.5987457294741916E-3</v>
+      </c>
+      <c r="AG16" s="2">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="AH16" s="4">
+        <v>1.6080564352140001E-3</v>
+      </c>
+      <c r="AI16" s="4">
+        <v>1.1668730299957211E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -967,8 +1226,28 @@
       <c r="X17" s="3">
         <v>4.6088108524219944</v>
       </c>
-    </row>
-    <row r="18" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB17" s="2">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="AC17" s="4">
+        <v>8.6272176049172742E-4</v>
+      </c>
+      <c r="AD17" s="4">
+        <v>5.3502305808586607E-3</v>
+      </c>
+      <c r="AG17" s="2">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="AH17" s="4">
+        <v>1.640805958059959E-3</v>
+      </c>
+      <c r="AI17" s="4">
+        <v>1.1037004752098321E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1009,8 +1288,28 @@
       <c r="X18" s="3">
         <v>4.4773674450766672</v>
       </c>
-    </row>
-    <row r="19" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB18" s="2">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="AC18" s="4">
+        <v>9.2209056998013446E-4</v>
+      </c>
+      <c r="AD18" s="4">
+        <v>6.664244090777649E-3</v>
+      </c>
+      <c r="AG18" s="2">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="AH18" s="4">
+        <v>1.548521025034724E-3</v>
+      </c>
+      <c r="AI18" s="4">
+        <v>1.202707670916035E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1051,8 +1350,28 @@
       <c r="X19" s="3">
         <v>4.5668297585573034</v>
       </c>
-    </row>
-    <row r="20" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB19" s="2">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="AC19" s="4">
+        <v>7.6493865361732644E-4</v>
+      </c>
+      <c r="AD19" s="4">
+        <v>9.1663036030846818E-3</v>
+      </c>
+      <c r="AG19" s="2">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="AH19" s="4">
+        <v>1.6367294083188719E-3</v>
+      </c>
+      <c r="AI19" s="4">
+        <v>1.133073590921419E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1093,8 +1412,28 @@
       <c r="X20" s="3">
         <v>3.846267516199017</v>
       </c>
-    </row>
-    <row r="21" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB20" s="2">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="AC20" s="4">
+        <v>8.5648234863549579E-4</v>
+      </c>
+      <c r="AD20" s="4">
+        <v>7.8483034925778804E-3</v>
+      </c>
+      <c r="AG20" s="2">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="AH20" s="4">
+        <v>1.606561883217893E-3</v>
+      </c>
+      <c r="AI20" s="4">
+        <v>1.163534975951085E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1135,8 +1474,28 @@
       <c r="X21" s="3">
         <v>4.2694943136476873</v>
       </c>
-    </row>
-    <row r="22" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB21" s="2">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="AC21" s="4">
+        <v>8.9941608027565895E-4</v>
+      </c>
+      <c r="AD21" s="4">
+        <v>5.8490371152067188E-3</v>
+      </c>
+      <c r="AG21" s="2">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="AH21" s="4">
+        <v>1.607627791773765E-3</v>
+      </c>
+      <c r="AI21" s="4">
+        <v>1.221373542034143E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1177,8 +1536,28 @@
       <c r="X22" s="3">
         <v>4.2540227088368434</v>
       </c>
-    </row>
-    <row r="23" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB22" s="2">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="AC22" s="4">
+        <v>9.6831375624059732E-4</v>
+      </c>
+      <c r="AD22" s="4">
+        <v>4.9253349369959383E-3</v>
+      </c>
+      <c r="AG22" s="2">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="AH22" s="4">
+        <v>1.6124582619833779E-3</v>
+      </c>
+      <c r="AI22" s="4">
+        <v>1.1001532099581589E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1219,8 +1598,28 @@
       <c r="X23" s="3">
         <v>2.9753045140627781</v>
       </c>
-    </row>
-    <row r="24" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB23" s="2">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="AC23" s="4">
+        <v>7.8706374006531313E-4</v>
+      </c>
+      <c r="AD23" s="4">
+        <v>7.0166700063517707E-3</v>
+      </c>
+      <c r="AG23" s="2">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="AH23" s="4">
+        <v>1.5553804431538421E-3</v>
+      </c>
+      <c r="AI23" s="4">
+        <v>1.29486321355248E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1261,8 +1660,28 @@
       <c r="X24" s="3">
         <v>3.6999609003665439</v>
       </c>
-    </row>
-    <row r="25" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB24" s="2">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="AC24" s="4">
+        <v>9.262975969762064E-4</v>
+      </c>
+      <c r="AD24" s="4">
+        <v>5.2188839667433066E-3</v>
+      </c>
+      <c r="AG24" s="2">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="AH24" s="4">
+        <v>1.6333281172912779E-3</v>
+      </c>
+      <c r="AI24" s="4">
+        <v>9.6698470551417007E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1303,8 +1722,28 @@
       <c r="X25" s="3">
         <v>4.4848966978115792</v>
       </c>
-    </row>
-    <row r="26" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB25" s="2">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="AC25" s="4">
+        <v>9.4145891132320825E-4</v>
+      </c>
+      <c r="AD25" s="4">
+        <v>5.1420285299677527E-3</v>
+      </c>
+      <c r="AG25" s="2">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="AH25" s="4">
+        <v>1.4718525935716661E-3</v>
+      </c>
+      <c r="AI25" s="4">
+        <v>1.433094594129678E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1345,8 +1784,28 @@
       <c r="X26" s="3">
         <v>3.4377345396641341</v>
       </c>
-    </row>
-    <row r="27" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB26" s="2">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="AC26" s="4">
+        <v>8.7841927228379997E-4</v>
+      </c>
+      <c r="AD26" s="4">
+        <v>4.9091243264284606E-3</v>
+      </c>
+      <c r="AG26" s="2">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="AH26" s="4">
+        <v>1.574066040174626E-3</v>
+      </c>
+      <c r="AI26" s="4">
+        <v>1.12911593622773E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1387,8 +1846,28 @@
       <c r="X27" s="3">
         <v>4.9737674891990524</v>
       </c>
-    </row>
-    <row r="28" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB27" s="2">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="AC27" s="4">
+        <v>8.4295102475085858E-4</v>
+      </c>
+      <c r="AD27" s="4">
+        <v>6.1897513399513026E-3</v>
+      </c>
+      <c r="AG27" s="2">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="AH27" s="4">
+        <v>1.596208708293438E-3</v>
+      </c>
+      <c r="AI27" s="4">
+        <v>1.263109211089136E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1429,8 +1908,28 @@
       <c r="X28" s="3">
         <v>3.073105460839145</v>
       </c>
-    </row>
-    <row r="29" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB28" s="2">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="AC28" s="4">
+        <v>8.9120654656589299E-4</v>
+      </c>
+      <c r="AD28" s="4">
+        <v>5.2295782136074376E-3</v>
+      </c>
+      <c r="AG28" s="2">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="AH28" s="4">
+        <v>1.6122918345138589E-3</v>
+      </c>
+      <c r="AI28" s="4">
+        <v>1.169752090444318E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1471,8 +1970,28 @@
       <c r="X29" s="3">
         <v>2.696476049129668</v>
       </c>
-    </row>
-    <row r="30" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB29" s="2">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="AC29" s="4">
+        <v>9.8355924384296552E-4</v>
+      </c>
+      <c r="AD29" s="4">
+        <v>4.4088195443491886E-3</v>
+      </c>
+      <c r="AG29" s="2">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="AH29" s="4">
+        <v>1.64138555503215E-3</v>
+      </c>
+      <c r="AI29" s="4">
+        <v>1.0928256309248379E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1513,8 +2032,28 @@
       <c r="X30" s="3">
         <v>4.8074296831338819</v>
       </c>
-    </row>
-    <row r="31" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB30" s="2">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="AC30" s="4">
+        <v>8.6127567909827739E-4</v>
+      </c>
+      <c r="AD30" s="4">
+        <v>6.8137955750758802E-3</v>
+      </c>
+      <c r="AG30" s="2">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="AH30" s="4">
+        <v>1.5821875492382041E-3</v>
+      </c>
+      <c r="AI30" s="4">
+        <v>1.300637867621721E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1555,8 +2094,28 @@
       <c r="X31" s="3">
         <v>5.5274363011843644</v>
       </c>
-    </row>
-    <row r="32" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB31" s="2">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="AC31" s="4">
+        <v>8.5793298368885677E-4</v>
+      </c>
+      <c r="AD31" s="4">
+        <v>8.3836850514006026E-3</v>
+      </c>
+      <c r="AG31" s="2">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="AH31" s="4">
+        <v>1.6216434678970901E-3</v>
+      </c>
+      <c r="AI31" s="4">
+        <v>1.0717621029435879E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1597,8 +2156,28 @@
       <c r="X32" s="3">
         <v>2.677210658524261</v>
       </c>
-    </row>
-    <row r="33" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB32" s="2">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="AC32" s="4">
+        <v>8.8296522610342048E-4</v>
+      </c>
+      <c r="AD32" s="4">
+        <v>6.254123444370035E-3</v>
+      </c>
+      <c r="AG32" s="2">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="AH32" s="4">
+        <v>1.627520779630746E-3</v>
+      </c>
+      <c r="AI32" s="4">
+        <v>1.1959081580324001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1639,8 +2218,28 @@
       <c r="X33" s="3">
         <v>3.840937615475625</v>
       </c>
-    </row>
-    <row r="34" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB33" s="2">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="AC33" s="4">
+        <v>8.8189256340739702E-4</v>
+      </c>
+      <c r="AD33" s="4">
+        <v>4.8209854126703283E-3</v>
+      </c>
+      <c r="AG33" s="2">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="AH33" s="4">
+        <v>1.5969104424504959E-3</v>
+      </c>
+      <c r="AI33" s="4">
+        <v>1.1945302913008941E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1681,8 +2280,28 @@
       <c r="X34" s="3">
         <v>3.632915572424074</v>
       </c>
-    </row>
-    <row r="35" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB34" s="2">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="AC34" s="4">
+        <v>9.1663038075533404E-4</v>
+      </c>
+      <c r="AD34" s="4">
+        <v>5.8413571107318787E-3</v>
+      </c>
+      <c r="AG34" s="2">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="AH34" s="4">
+        <v>1.624925857497886E-3</v>
+      </c>
+      <c r="AI34" s="4">
+        <v>1.1039960771697971E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1723,8 +2342,28 @@
       <c r="X35" s="3">
         <v>4.5555272851891191</v>
       </c>
-    </row>
-    <row r="36" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB35" s="2">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="AC35" s="4">
+        <v>7.8899438645142642E-4</v>
+      </c>
+      <c r="AD35" s="4">
+        <v>9.4701684497667579E-3</v>
+      </c>
+      <c r="AG35" s="2">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="AH35" s="4">
+        <v>1.6172003450377231E-3</v>
+      </c>
+      <c r="AI35" s="4">
+        <v>1.077857663578146E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1765,8 +2404,28 @@
       <c r="X36" s="3">
         <v>3.0035977046396289</v>
       </c>
-    </row>
-    <row r="37" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB36" s="2">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="AC36" s="4">
+        <v>8.6187439991011533E-4</v>
+      </c>
+      <c r="AD36" s="4">
+        <v>5.383488897508692E-3</v>
+      </c>
+      <c r="AG36" s="2">
+        <f t="shared" si="5"/>
+        <v>31</v>
+      </c>
+      <c r="AH36" s="4">
+        <v>1.592824211903438E-3</v>
+      </c>
+      <c r="AI36" s="4">
+        <v>1.1484634747663151E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1807,8 +2466,28 @@
       <c r="X37" s="3">
         <v>5.0844061253919</v>
       </c>
-    </row>
-    <row r="38" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB37" s="2">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="AC37" s="4">
+        <v>8.1945664294456487E-4</v>
+      </c>
+      <c r="AD37" s="4">
+        <v>8.8199934821025817E-3</v>
+      </c>
+      <c r="AG37" s="2">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="AH37" s="4">
+        <v>1.624584292388515E-3</v>
+      </c>
+      <c r="AI37" s="4">
+        <v>1.138742636756657E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1849,8 +2528,28 @@
       <c r="X38" s="3">
         <v>5.1551411021819762</v>
       </c>
-    </row>
-    <row r="39" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB38" s="2">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="AC38" s="4">
+        <v>7.8407001413694649E-4</v>
+      </c>
+      <c r="AD38" s="4">
+        <v>7.9862340409000299E-3</v>
+      </c>
+      <c r="AG38" s="2">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
+      <c r="AH38" s="4">
+        <v>1.55238280873726E-3</v>
+      </c>
+      <c r="AI38" s="4">
+        <v>1.281028832348245E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1891,8 +2590,28 @@
       <c r="X39" s="3">
         <v>3.834765503059899</v>
       </c>
-    </row>
-    <row r="40" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB39" s="2">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="AC39" s="4">
+        <v>8.9696083082663148E-4</v>
+      </c>
+      <c r="AD39" s="4">
+        <v>5.5065293687982806E-3</v>
+      </c>
+      <c r="AG39" s="2">
+        <f t="shared" si="5"/>
+        <v>34</v>
+      </c>
+      <c r="AH39" s="4">
+        <v>1.658049013577637E-3</v>
+      </c>
+      <c r="AI39" s="4">
+        <v>1.0467945202287981E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1933,8 +2652,28 @@
       <c r="X40" s="3">
         <v>2.9032988054437441</v>
       </c>
-    </row>
-    <row r="41" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB40" s="2">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="AC40" s="4">
+        <v>9.1559517486767086E-4</v>
+      </c>
+      <c r="AD40" s="4">
+        <v>6.3514971919654212E-3</v>
+      </c>
+      <c r="AG40" s="2">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="AH40" s="4">
+        <v>1.63421256638833E-3</v>
+      </c>
+      <c r="AI40" s="4">
+        <v>1.074212064642795E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1975,8 +2714,28 @@
       <c r="X41" s="3">
         <v>4.0096773780429444</v>
       </c>
-    </row>
-    <row r="42" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB41" s="2">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="AC41" s="4">
+        <v>8.8953667395526368E-4</v>
+      </c>
+      <c r="AD41" s="4">
+        <v>6.2632808780881226E-3</v>
+      </c>
+      <c r="AG41" s="2">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="AH41" s="4">
+        <v>1.6273757434877171E-3</v>
+      </c>
+      <c r="AI41" s="4">
+        <v>1.123049429650283E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2017,8 +2776,28 @@
       <c r="X42" s="3">
         <v>3.951779108007095</v>
       </c>
-    </row>
-    <row r="43" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB42" s="2">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="AC42" s="4">
+        <v>8.5012328763200181E-4</v>
+      </c>
+      <c r="AD42" s="4">
+        <v>7.5876136563189757E-3</v>
+      </c>
+      <c r="AG42" s="2">
+        <f t="shared" si="5"/>
+        <v>37</v>
+      </c>
+      <c r="AH42" s="4">
+        <v>1.5857870370929181E-3</v>
+      </c>
+      <c r="AI42" s="4">
+        <v>1.2086237487118481E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2059,8 +2838,28 @@
       <c r="X43" s="3">
         <v>4.7645145961785964</v>
       </c>
-    </row>
-    <row r="44" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB43" s="2">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="AC43" s="4">
+        <v>8.2471618472576048E-4</v>
+      </c>
+      <c r="AD43" s="4">
+        <v>8.2139286633500612E-3</v>
+      </c>
+      <c r="AG43" s="2">
+        <f t="shared" si="5"/>
+        <v>38</v>
+      </c>
+      <c r="AH43" s="4">
+        <v>1.677802970332765E-3</v>
+      </c>
+      <c r="AI43" s="4">
+        <v>1.025914370528767E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2101,8 +2900,28 @@
       <c r="X44" s="3">
         <v>2.7834375856302729</v>
       </c>
-    </row>
-    <row r="45" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB44" s="2">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="AC44" s="4">
+        <v>9.2322797262964999E-4</v>
+      </c>
+      <c r="AD44" s="4">
+        <v>5.0740876061628774E-3</v>
+      </c>
+      <c r="AG44" s="2">
+        <f t="shared" si="5"/>
+        <v>39</v>
+      </c>
+      <c r="AH44" s="4">
+        <v>1.6649925385162009E-3</v>
+      </c>
+      <c r="AI44" s="4">
+        <v>9.9195117481252707E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2143,8 +2962,28 @@
       <c r="X45" s="3">
         <v>4.3890422515964866</v>
       </c>
-    </row>
-    <row r="46" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB45" s="2">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="AC45" s="4">
+        <v>8.3189701341573408E-4</v>
+      </c>
+      <c r="AD45" s="4">
+        <v>7.9173543524065151E-3</v>
+      </c>
+      <c r="AG45" s="2">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="AH45" s="4">
+        <v>1.607291445532746E-3</v>
+      </c>
+      <c r="AI45" s="4">
+        <v>1.115160381169138E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2185,8 +3024,28 @@
       <c r="X46" s="3">
         <v>3.7014409129817172</v>
       </c>
-    </row>
-    <row r="47" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB46" s="2">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="AC46" s="4">
+        <v>8.4725194294970696E-4</v>
+      </c>
+      <c r="AD46" s="4">
+        <v>8.6944695513224059E-3</v>
+      </c>
+      <c r="AG46" s="2">
+        <f t="shared" si="5"/>
+        <v>41</v>
+      </c>
+      <c r="AH46" s="4">
+        <v>1.6480089667861731E-3</v>
+      </c>
+      <c r="AI46" s="4">
+        <v>1.079947686843208E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2227,8 +3086,28 @@
       <c r="X47" s="3">
         <v>4.1042147526753832</v>
       </c>
-    </row>
-    <row r="48" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB47" s="2">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="AC47" s="4">
+        <v>9.2248137705867438E-4</v>
+      </c>
+      <c r="AD47" s="4">
+        <v>4.5614777306711802E-3</v>
+      </c>
+      <c r="AG47" s="2">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+      <c r="AH47" s="4">
+        <v>1.6303115349053409E-3</v>
+      </c>
+      <c r="AI47" s="4">
+        <v>1.165194618295187E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2269,8 +3148,28 @@
       <c r="X48" s="3">
         <v>3.2643453663718018</v>
       </c>
-    </row>
-    <row r="49" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB48" s="2">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="AC48" s="4">
+        <v>8.1927442868793329E-4</v>
+      </c>
+      <c r="AD48" s="4">
+        <v>7.5480578593691474E-3</v>
+      </c>
+      <c r="AG48" s="2">
+        <f t="shared" si="5"/>
+        <v>43</v>
+      </c>
+      <c r="AH48" s="4">
+        <v>1.648044340137864E-3</v>
+      </c>
+      <c r="AI48" s="4">
+        <v>1.1122546973785209E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2311,8 +3210,28 @@
       <c r="X49" s="3">
         <v>4.1109743231738456</v>
       </c>
-    </row>
-    <row r="50" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB49" s="2">
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+      <c r="AC49" s="4">
+        <v>9.6845776757179078E-4</v>
+      </c>
+      <c r="AD49" s="4">
+        <v>4.514784686722886E-3</v>
+      </c>
+      <c r="AG49" s="2">
+        <f t="shared" si="5"/>
+        <v>44</v>
+      </c>
+      <c r="AH49" s="4">
+        <v>1.583199112964653E-3</v>
+      </c>
+      <c r="AI49" s="4">
+        <v>1.245908013866423E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2353,8 +3272,28 @@
       <c r="X50" s="3">
         <v>3.4518841112354508</v>
       </c>
-    </row>
-    <row r="51" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB50" s="2">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="AC50" s="4">
+        <v>8.2732407862393781E-4</v>
+      </c>
+      <c r="AD50" s="4">
+        <v>8.2313946872629527E-3</v>
+      </c>
+      <c r="AG50" s="2">
+        <f t="shared" si="5"/>
+        <v>45</v>
+      </c>
+      <c r="AH50" s="4">
+        <v>1.594791490307647E-3</v>
+      </c>
+      <c r="AI50" s="4">
+        <v>1.1358352020879659E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2395,8 +3334,28 @@
       <c r="X51" s="3">
         <v>2.7167201169501691</v>
       </c>
-    </row>
-    <row r="52" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB51" s="2">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="AC51" s="4">
+        <v>9.239102621895587E-4</v>
+      </c>
+      <c r="AD51" s="4">
+        <v>5.6084003604215463E-3</v>
+      </c>
+      <c r="AG51" s="2">
+        <f t="shared" si="5"/>
+        <v>46</v>
+      </c>
+      <c r="AH51" s="4">
+        <v>1.6910161683128761E-3</v>
+      </c>
+      <c r="AI51" s="4">
+        <v>1.0522406086421821E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2437,8 +3396,28 @@
       <c r="X52" s="3">
         <v>2.8181934435852911</v>
       </c>
-    </row>
-    <row r="53" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB52" s="2">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="AC52" s="4">
+        <v>9.6177525790612094E-4</v>
+      </c>
+      <c r="AD52" s="4">
+        <v>5.2829536118410899E-3</v>
+      </c>
+      <c r="AG52" s="2">
+        <f t="shared" si="5"/>
+        <v>47</v>
+      </c>
+      <c r="AH52" s="4">
+        <v>1.6039527538146421E-3</v>
+      </c>
+      <c r="AI52" s="4">
+        <v>1.1154338827969399E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2479,8 +3458,28 @@
       <c r="X53" s="3">
         <v>3.180311417306005</v>
       </c>
-    </row>
-    <row r="54" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB53" s="2">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="AC53" s="4">
+        <v>9.19886194547712E-4</v>
+      </c>
+      <c r="AD53" s="4">
+        <v>4.7247065064285367E-3</v>
+      </c>
+      <c r="AG53" s="2">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="AH53" s="4">
+        <v>1.616307846401713E-3</v>
+      </c>
+      <c r="AI53" s="4">
+        <v>1.1024238762191149E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2521,8 +3520,28 @@
       <c r="X54" s="3">
         <v>3.5987215751012571</v>
       </c>
-    </row>
-    <row r="55" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB54" s="2">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="AC54" s="4">
+        <v>8.8049758828907766E-4</v>
+      </c>
+      <c r="AD54" s="4">
+        <v>5.9240492335451431E-3</v>
+      </c>
+      <c r="AG54" s="2">
+        <f t="shared" si="5"/>
+        <v>49</v>
+      </c>
+      <c r="AH54" s="4">
+        <v>1.6131370402637671E-3</v>
+      </c>
+      <c r="AI54" s="4">
+        <v>1.1789664935226291E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D55" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2563,8 +3582,28 @@
       <c r="X55" s="3">
         <v>3.9341105574149</v>
       </c>
-    </row>
-    <row r="57" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB55" s="2">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="AC55" s="4">
+        <v>9.1830921364576522E-4</v>
+      </c>
+      <c r="AD55" s="4">
+        <v>4.9328516840289769E-3</v>
+      </c>
+      <c r="AG55" s="2">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="AH55" s="4">
+        <v>1.629940881822607E-3</v>
+      </c>
+      <c r="AI55" s="4">
+        <v>1.0213244504360199E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>4</v>
       </c>
@@ -2609,8 +3648,30 @@
         <f>AVERAGE(X6:X55)</f>
         <v>3.759815268950069</v>
       </c>
-    </row>
-    <row r="58" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="AB57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC57" s="4">
+        <f>AVERAGE(AC6:AC55)</f>
+        <v>8.8132614522225673E-4</v>
+      </c>
+      <c r="AD57" s="4">
+        <f>AVERAGE(AD6:AD55)</f>
+        <v>6.3054894442772114E-3</v>
+      </c>
+      <c r="AG57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH57" s="4">
+        <f>AVERAGE(AH6:AH55)</f>
+        <v>1.6159746629849192E-3</v>
+      </c>
+      <c r="AI57" s="4">
+        <f>AVERAGE(AI6:AI55)</f>
+        <v>1.1370663961253143E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="4:35" x14ac:dyDescent="0.25">
       <c r="D58" s="2" t="s">
         <v>5</v>
       </c>
@@ -2655,8 +3716,31 @@
         <f>_xlfn.STDEV.S(X6:X55)</f>
         <v>0.73228288979503398</v>
       </c>
+      <c r="AB58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC58" s="4">
+        <f>_xlfn.STDEV.S(AC6:AC55)</f>
+        <v>5.2597398990294191E-5</v>
+      </c>
+      <c r="AD58" s="4">
+        <f>_xlfn.STDEV.S(AD6:AD55)</f>
+        <v>1.3820977348093018E-3</v>
+      </c>
+      <c r="AG58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH58" s="4">
+        <f>_xlfn.STDEV.S(AH6:AH55)</f>
+        <v>4.3343039666225736E-5</v>
+      </c>
+      <c r="AI58" s="4">
+        <f>_xlfn.STDEV.S(AI6:AI55)</f>
+        <v>9.9190554967681357E-4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>